<commit_message>
Fixed a lot of bugs.
</commit_message>
<xml_diff>
--- a/RougueQuest - Items and Enemies.xlsx
+++ b/RougueQuest - Items and Enemies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NTDLS\RougueQuest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C166ABDF-67F6-45A7-A51D-914A1B809A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973A72F6-5912-4F52-825F-33AFFF234198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5415" yWindow="795" windowWidth="15075" windowHeight="9615" activeTab="2" xr2:uid="{C202AA48-B5B6-42E9-AECB-65F2B3A7610F}"/>
+    <workbookView xWindow="5415" yWindow="795" windowWidth="15075" windowHeight="9615" xr2:uid="{C202AA48-B5B6-42E9-AECB-65F2B3A7610F}"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="95">
   <si>
     <t>Name</t>
   </si>
@@ -191,9 +191,6 @@
     <t>1d6+2</t>
   </si>
   <si>
-    <t>Short Sword +3</t>
-  </si>
-  <si>
     <t>1d6+3</t>
   </si>
   <si>
@@ -291,6 +288,30 @@
   </si>
   <si>
     <t>Cloak of Protection +2</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Broad Sword +2</t>
+  </si>
+  <si>
+    <t>1d9+2</t>
+  </si>
+  <si>
+    <t>1d5+1</t>
+  </si>
+  <si>
+    <t>1d5+2</t>
+  </si>
+  <si>
+    <t>Mace +1</t>
+  </si>
+  <si>
+    <t>Mace +2</t>
+  </si>
+  <si>
+    <t>Short Sword +5</t>
   </si>
 </sst>
 </file>
@@ -334,9 +355,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -651,551 +684,705 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAA9A541-9445-4B26-B43F-4615F42143DC}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2">
+        <v>105</v>
+      </c>
+      <c r="E2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
+      <c r="E3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="C2">
+      <c r="D4">
         <v>20</v>
       </c>
-      <c r="D2">
+      <c r="E4">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="C3">
+      <c r="D5">
         <v>20</v>
       </c>
-      <c r="D3">
+      <c r="E5">
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="C4">
+      <c r="D6">
         <v>30</v>
       </c>
-      <c r="D4">
+      <c r="E6">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7">
+        <v>110</v>
+      </c>
+      <c r="E7">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8">
+        <v>100</v>
+      </c>
+      <c r="E8">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="C5">
+      <c r="D9">
         <v>40</v>
       </c>
-      <c r="D5">
+      <c r="E9">
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
         <v>20</v>
       </c>
-      <c r="C6">
+      <c r="D10">
         <v>50</v>
       </c>
-      <c r="D6">
+      <c r="E10">
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
         <v>22</v>
       </c>
-      <c r="C7">
+      <c r="D11">
         <v>50</v>
       </c>
-      <c r="D7">
+      <c r="E11">
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12">
+        <v>50</v>
+      </c>
+      <c r="E12">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
         <v>24</v>
       </c>
-      <c r="C8">
+      <c r="D13">
         <v>10</v>
       </c>
-      <c r="D8">
+      <c r="E13">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>25</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
         <v>26</v>
       </c>
-      <c r="C9">
+      <c r="D14">
         <v>15</v>
       </c>
-      <c r="D9">
+      <c r="E14">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>27</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
         <v>28</v>
       </c>
-      <c r="C10">
+      <c r="D15">
         <v>5</v>
       </c>
-      <c r="D10">
+      <c r="E15">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16">
+        <v>120</v>
+      </c>
+      <c r="E16">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
         <v>30</v>
       </c>
-      <c r="C11">
+      <c r="D17">
         <v>25</v>
       </c>
-      <c r="D11">
+      <c r="E17">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>31</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
         <v>12</v>
       </c>
-      <c r="C12">
+      <c r="D18">
         <v>16</v>
       </c>
-      <c r="D12">
+      <c r="E18">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19">
+        <v>110</v>
+      </c>
+      <c r="E19">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>32</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
         <v>18</v>
       </c>
-      <c r="C13">
+      <c r="D20">
         <v>50</v>
       </c>
-      <c r="D13">
+      <c r="E20">
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>33</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
         <v>20</v>
-      </c>
-      <c r="C14">
-        <v>60</v>
-      </c>
-      <c r="D14">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15">
-        <v>20</v>
-      </c>
-      <c r="D15">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16">
-        <v>80</v>
-      </c>
-      <c r="D16">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17">
-        <v>85</v>
-      </c>
-      <c r="D17">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18">
-        <v>20</v>
-      </c>
-      <c r="D18">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19">
-        <v>20</v>
-      </c>
-      <c r="D19">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20">
-        <v>20</v>
-      </c>
-      <c r="D20">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21">
-        <v>25</v>
       </c>
       <c r="D21">
         <v>60</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22">
+        <v>20</v>
+      </c>
+      <c r="E22">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23">
+        <v>80</v>
+      </c>
+      <c r="E23">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24">
+        <v>85</v>
+      </c>
+      <c r="E24">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25">
+        <v>20</v>
+      </c>
+      <c r="E25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26">
+        <v>20</v>
+      </c>
+      <c r="E26">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27">
+        <v>20</v>
+      </c>
+      <c r="E27">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28">
+        <v>25</v>
+      </c>
+      <c r="E28">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29">
+        <v>25</v>
+      </c>
+      <c r="E29">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30">
+        <v>25</v>
+      </c>
+      <c r="E30">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>45</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
         <v>28</v>
       </c>
-      <c r="C22">
+      <c r="D31">
         <v>25</v>
       </c>
-      <c r="D22">
+      <c r="E31">
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>46</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
         <v>16</v>
       </c>
-      <c r="C23">
+      <c r="D32">
         <v>55</v>
       </c>
-      <c r="D23">
+      <c r="E32">
         <v>110</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>47</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
         <v>12</v>
       </c>
-      <c r="C24">
+      <c r="D33">
         <v>60</v>
       </c>
-      <c r="D24">
+      <c r="E33">
         <v>115</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>48</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
         <v>49</v>
       </c>
-      <c r="C25">
+      <c r="D34">
         <v>15</v>
       </c>
-      <c r="D25">
+      <c r="E34">
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>50</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
         <v>51</v>
       </c>
-      <c r="C26">
+      <c r="D35">
         <v>15</v>
       </c>
-      <c r="D26">
+      <c r="E35">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>52</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
         <v>53</v>
       </c>
-      <c r="C27">
+      <c r="D36">
         <v>15</v>
       </c>
-      <c r="D27">
+      <c r="E36">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>94</v>
+      </c>
+      <c r="B37">
+        <v>5</v>
+      </c>
+      <c r="C37" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37">
         <v>15</v>
       </c>
-      <c r="D28">
+      <c r="E37">
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29">
-        <v>15</v>
-      </c>
-      <c r="D29">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30">
-        <v>105</v>
-      </c>
-      <c r="D30">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>58</v>
-      </c>
-      <c r="B31" t="s">
-        <v>59</v>
-      </c>
-      <c r="C31">
-        <v>100</v>
-      </c>
-      <c r="D31">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32">
-        <v>110</v>
-      </c>
-      <c r="D32">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>62</v>
-      </c>
-      <c r="B33" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33">
-        <v>100</v>
-      </c>
-      <c r="D33">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34">
-        <v>120</v>
-      </c>
-      <c r="D34">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>67</v>
       </c>
-      <c r="C35">
-        <v>110</v>
-      </c>
-      <c r="D35">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38">
+        <v>18</v>
+      </c>
+      <c r="E38">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>68</v>
       </c>
-      <c r="B36" t="s">
-        <v>12</v>
-      </c>
-      <c r="C36">
-        <v>18</v>
-      </c>
-      <c r="D36">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39">
+        <v>25</v>
+      </c>
+      <c r="E39">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>69</v>
       </c>
-      <c r="B37" t="s">
-        <v>26</v>
-      </c>
-      <c r="C37">
-        <v>25</v>
-      </c>
-      <c r="D37">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>70</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
         <v>28</v>
       </c>
-      <c r="C38">
+      <c r="D40">
         <v>10</v>
       </c>
-      <c r="D38">
+      <c r="E40">
         <v>10</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E40">
+    <sortCondition ref="A2:A40"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -1203,369 +1390,431 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2CC720-2AFD-489A-814E-D75EB644CEB6}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>40</v>
+      </c>
+      <c r="D2">
+        <v>16</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>40</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2">
+      <c r="B6" s="5">
+        <v>3</v>
+      </c>
+      <c r="C6">
         <v>150</v>
-      </c>
-      <c r="C2">
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <v>25</v>
-      </c>
-      <c r="E2">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3">
-        <v>200</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>16</v>
-      </c>
-      <c r="E3">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4">
-        <v>600</v>
-      </c>
-      <c r="C4">
-        <v>28</v>
-      </c>
-      <c r="D4">
-        <v>30</v>
-      </c>
-      <c r="E4">
-        <v>30</v>
-      </c>
-      <c r="F4" t="s">
-        <v>79</v>
-      </c>
-      <c r="G4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5">
-        <v>250</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>8</v>
-      </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6">
-        <v>60</v>
-      </c>
-      <c r="C6">
-        <v>16</v>
       </c>
       <c r="D6">
         <v>20</v>
       </c>
       <c r="E6">
+        <v>25</v>
+      </c>
+      <c r="F6">
+        <v>16</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="5">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>200</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>16</v>
+      </c>
+      <c r="F7">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="5">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>250</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
         <v>8</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="5">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>600</v>
+      </c>
+      <c r="D9">
+        <v>28</v>
+      </c>
+      <c r="E9">
         <v>30</v>
       </c>
-      <c r="G6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7">
-        <v>20</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7">
-        <v>5</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>83</v>
-      </c>
-      <c r="B8">
-        <v>40</v>
-      </c>
-      <c r="C8">
-        <v>6</v>
-      </c>
-      <c r="D8">
-        <v>10</v>
-      </c>
-      <c r="E8">
-        <v>5</v>
-      </c>
-      <c r="F8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B9">
+      <c r="F9">
         <v>30</v>
       </c>
-      <c r="C9">
-        <v>5</v>
-      </c>
-      <c r="D9">
-        <v>5</v>
-      </c>
-      <c r="E9">
-        <v>3</v>
-      </c>
-      <c r="F9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9">
-        <v>4</v>
+      <c r="G9" t="s">
+        <v>78</v>
+      </c>
+      <c r="H9">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H9">
+    <sortCondition ref="B2:B9"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75747614-1788-425D-A945-26690DAA4255}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+      <c r="B1" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>11</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>50</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>240</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3">
         <v>0</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>15</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>1</v>
       </c>
       <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
         <v>8</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6">
         <v>2</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>20</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>85</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
+      <c r="B8" s="3">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
         <v>8</v>
       </c>
-      <c r="D7">
+      <c r="E8">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>86</v>
       </c>
-      <c r="B8">
+      <c r="B9" s="3">
         <v>2</v>
       </c>
-      <c r="C8">
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
         <v>8</v>
       </c>
-      <c r="D8">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <v>8</v>
-      </c>
-      <c r="D9">
+      <c r="E9">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed issue with cloned metadata
</commit_message>
<xml_diff>
--- a/RougueQuest - Items and Enemies.xlsx
+++ b/RougueQuest - Items and Enemies.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NTDLS\RougueQuest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8BC3E5-882C-44DB-9A15-25390D24BB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC7806CF-C873-4CC7-B836-F0DDC870B1F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9312" yWindow="216" windowWidth="12312" windowHeight="13260" activeTab="1" xr2:uid="{C202AA48-B5B6-42E9-AECB-65F2B3A7610F}"/>
+    <workbookView xWindow="-5184" yWindow="5304" windowWidth="12312" windowHeight="13260" activeTab="1" xr2:uid="{C202AA48-B5B6-42E9-AECB-65F2B3A7610F}"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
-    <sheet name="Potion" sheetId="4" r:id="rId2"/>
-    <sheet name="Enemies" sheetId="3" r:id="rId3"/>
-    <sheet name="Armor" sheetId="2" r:id="rId4"/>
+    <sheet name="Projectiles" sheetId="5" r:id="rId2"/>
+    <sheet name="Potion" sheetId="4" r:id="rId3"/>
+    <sheet name="Enemies" sheetId="3" r:id="rId4"/>
+    <sheet name="Armor" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="124">
   <si>
     <t>Name</t>
   </si>
@@ -385,6 +386,21 @@
   </si>
   <si>
     <t>Strength +5, 1 hour</t>
+  </si>
+  <si>
+    <t>Wooden Arrow</t>
+  </si>
+  <si>
+    <t>Steel Arrow</t>
+  </si>
+  <si>
+    <t>Silver Arrow</t>
+  </si>
+  <si>
+    <t>2d3</t>
+  </si>
+  <si>
+    <t>Flaming Arrow</t>
   </si>
 </sst>
 </file>
@@ -760,7 +776,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="E11" sqref="E11:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1583,10 +1599,133 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75064B25-7A11-4247-9878-09501A5C4D02}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61CAF6BD-7DF9-4703-AB96-7954B9A63A6D}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1734,7 +1873,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2CC720-2AFD-489A-814E-D75EB644CEB6}">
   <dimension ref="A1:H9"/>
   <sheetViews>
@@ -1994,7 +2133,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75747614-1788-425D-A945-26690DAA4255}">
   <dimension ref="A1:F9"/>
   <sheetViews>

</xml_diff>

<commit_message>
Item reorg, fixed inventory moving and store entering.
</commit_message>
<xml_diff>
--- a/RougueQuest - Items and Enemies.xlsx
+++ b/RougueQuest - Items and Enemies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NTDLS\RougueQuest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931683EA-9348-41CF-B86D-6D2A33E0EE76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3050868A-314F-4F84-9BCF-45D61CA235FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7764" yWindow="2328" windowWidth="17004" windowHeight="13356" xr2:uid="{C202AA48-B5B6-42E9-AECB-65F2B3A7610F}"/>
+    <workbookView xWindow="0" yWindow="588" windowWidth="17004" windowHeight="13356" xr2:uid="{C202AA48-B5B6-42E9-AECB-65F2B3A7610F}"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -894,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAA9A541-9445-4B26-B43F-4615F42143DC}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1860,7 +1860,7 @@
         <v>159</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D42" s="7">
         <v>1</v>

</xml_diff>

<commit_message>
Added scrolls and splash damage.
</commit_message>
<xml_diff>
--- a/RougueQuest - Items and Enemies.xlsx
+++ b/RougueQuest - Items and Enemies.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NTDLS\RougueQuest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3050868A-314F-4F84-9BCF-45D61CA235FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079D1A39-2E16-49F2-B30D-82AE67CE3287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="588" windowWidth="17004" windowHeight="13356" xr2:uid="{C202AA48-B5B6-42E9-AECB-65F2B3A7610F}"/>
+    <workbookView xWindow="804" yWindow="972" windowWidth="17004" windowHeight="13356" activeTab="1" xr2:uid="{C202AA48-B5B6-42E9-AECB-65F2B3A7610F}"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
-    <sheet name="Projectiles" sheetId="5" r:id="rId2"/>
-    <sheet name="Potion" sheetId="4" r:id="rId3"/>
-    <sheet name="Wands" sheetId="7" r:id="rId4"/>
-    <sheet name="Enemies" sheetId="3" r:id="rId5"/>
-    <sheet name="Armor" sheetId="2" r:id="rId6"/>
-    <sheet name="Misc." sheetId="6" r:id="rId7"/>
+    <sheet name="Spells" sheetId="8" r:id="rId2"/>
+    <sheet name="Projectiles" sheetId="5" r:id="rId3"/>
+    <sheet name="Potion" sheetId="4" r:id="rId4"/>
+    <sheet name="Wands" sheetId="7" r:id="rId5"/>
+    <sheet name="Enemies" sheetId="3" r:id="rId6"/>
+    <sheet name="Armor" sheetId="2" r:id="rId7"/>
+    <sheet name="Misc." sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="162">
   <si>
     <t>Name</t>
   </si>
@@ -514,13 +515,16 @@
   </si>
   <si>
     <t>Composite Bow</t>
+  </si>
+  <si>
+    <t>https://strategywiki.org/wiki/Castle_of_the_Winds/Magic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -532,6 +536,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -554,10 +566,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -578,8 +591,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -894,7 +909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAA9A541-9445-4B26-B43F-4615F42143DC}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
@@ -1885,6 +1900,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23A5046-8B05-44D0-A4EA-E6B6EFAC6BD3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{1C5A6357-8CB1-4B74-B6E0-9568922B8B5D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75064B25-7A11-4247-9878-09501A5C4D02}">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -2005,7 +2043,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61CAF6BD-7DF9-4703-AB96-7954B9A63A6D}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -2155,7 +2193,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A87D24B-7889-450E-B5C6-B6D3B829E5B0}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2202,7 +2240,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2CC720-2AFD-489A-814E-D75EB644CEB6}">
   <dimension ref="A1:H9"/>
   <sheetViews>
@@ -2462,7 +2500,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75747614-1788-425D-A945-26690DAA4255}">
   <dimension ref="A1:F17"/>
   <sheetViews>
@@ -2823,7 +2861,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E46510A5-96DE-4B16-B264-64B8352FBAF2}">
   <dimension ref="A1:F13"/>
   <sheetViews>

</xml_diff>

<commit_message>
New enemies, new items, new animations, new bugs.
</commit_message>
<xml_diff>
--- a/RougueQuest - Items and Enemies.xlsx
+++ b/RougueQuest - Items and Enemies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NTDLS\RougueQuest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F527AD-E95C-40DF-BE58-6FC694491E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C59194-0CB0-475F-A55B-8CB351BEBC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14160" activeTab="5" xr2:uid="{C202AA48-B5B6-42E9-AECB-65F2B3A7610F}"/>
+    <workbookView xWindow="2700" yWindow="336" windowWidth="17004" windowHeight="13356" activeTab="5" xr2:uid="{C202AA48-B5B6-42E9-AECB-65F2B3A7610F}"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -22,17 +22,26 @@
     <sheet name="Armor" sheetId="2" r:id="rId7"/>
     <sheet name="Misc." sheetId="6" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="187">
   <si>
     <t>Name</t>
   </si>
@@ -259,9 +268,6 @@
     <t>Black Bear</t>
   </si>
   <si>
-    <t>2d12</t>
-  </si>
-  <si>
     <t>Demon Fighter Major</t>
   </si>
   <si>
@@ -559,13 +565,43 @@
     <t>Electric Golem</t>
   </si>
   <si>
-    <t>Stone Golem</t>
-  </si>
-  <si>
     <t>Ice</t>
   </si>
   <si>
     <t>Electric</t>
+  </si>
+  <si>
+    <t>Fire Golem</t>
+  </si>
+  <si>
+    <t>Earth Golem</t>
+  </si>
+  <si>
+    <t>Earth</t>
+  </si>
+  <si>
+    <t>Earth Centipede</t>
+  </si>
+  <si>
+    <t>Electric Centipede</t>
+  </si>
+  <si>
+    <t>Fire Centipede</t>
+  </si>
+  <si>
+    <t>Ice Centipede</t>
+  </si>
+  <si>
+    <t>Giant Fire Ant</t>
+  </si>
+  <si>
+    <t>Giant Earth Ant</t>
+  </si>
+  <si>
+    <t>Giant Electric Ant</t>
+  </si>
+  <si>
+    <t>Giant Ice Ant</t>
   </si>
 </sst>
 </file>
@@ -609,7 +645,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -629,6 +665,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -964,13 +1006,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>8</v>
@@ -982,7 +1024,7 @@
         <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -990,7 +1032,7 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1013,7 +1055,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D3">
         <v>6</v>
@@ -1036,7 +1078,7 @@
         <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -1059,7 +1101,7 @@
         <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D5">
         <v>10</v>
@@ -1082,7 +1124,7 @@
         <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1105,7 +1147,7 @@
         <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1128,7 +1170,7 @@
         <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1151,7 +1193,7 @@
         <v>68</v>
       </c>
       <c r="B9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1174,7 +1216,7 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1197,7 +1239,7 @@
         <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1220,7 +1262,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1243,7 +1285,7 @@
         <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1266,7 +1308,7 @@
         <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1289,7 +1331,7 @@
         <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1312,7 +1354,7 @@
         <v>66</v>
       </c>
       <c r="B16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1332,16 +1374,16 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D17">
         <v>2</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F17">
         <v>25</v>
@@ -1355,16 +1397,16 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D18">
         <v>2</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F18">
         <v>25</v>
@@ -1381,7 +1423,7 @@
         <v>47</v>
       </c>
       <c r="B19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -1404,7 +1446,7 @@
         <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -1427,7 +1469,7 @@
         <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D21">
         <v>3</v>
@@ -1447,10 +1489,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D22">
         <v>5</v>
@@ -1473,7 +1515,7 @@
         <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D23">
         <v>3</v>
@@ -1496,7 +1538,7 @@
         <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D24">
         <v>3</v>
@@ -1519,7 +1561,7 @@
         <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D25">
         <v>3</v>
@@ -1542,7 +1584,7 @@
         <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D26">
         <v>5</v>
@@ -1565,7 +1607,7 @@
         <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D27">
         <v>5</v>
@@ -1588,7 +1630,7 @@
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D28">
         <v>3</v>
@@ -1611,7 +1653,7 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D29">
         <v>3</v>
@@ -1634,7 +1676,7 @@
         <v>18</v>
       </c>
       <c r="B30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D30">
         <v>3</v>
@@ -1657,7 +1699,7 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D31">
         <v>3</v>
@@ -1680,7 +1722,7 @@
         <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D32">
         <v>5</v>
@@ -1700,16 +1742,16 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D33">
         <v>6</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F33">
         <v>50</v>
@@ -1726,7 +1768,7 @@
         <v>64</v>
       </c>
       <c r="B34" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D34">
         <v>18</v>
@@ -1749,7 +1791,7 @@
         <v>28</v>
       </c>
       <c r="B35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D35">
         <v>5</v>
@@ -1772,7 +1814,7 @@
         <v>12</v>
       </c>
       <c r="B36" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D36">
         <v>5</v>
@@ -1795,7 +1837,7 @@
         <v>54</v>
       </c>
       <c r="B37" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D37">
         <v>20</v>
@@ -1818,7 +1860,7 @@
         <v>62</v>
       </c>
       <c r="B38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D38">
         <v>28</v>
@@ -1841,7 +1883,7 @@
         <v>60</v>
       </c>
       <c r="B39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D39">
         <v>25</v>
@@ -1864,7 +1906,7 @@
         <v>56</v>
       </c>
       <c r="B40" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D40">
         <v>30</v>
@@ -1884,10 +1926,10 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>146</v>
+      </c>
+      <c r="B41" t="s">
         <v>147</v>
-      </c>
-      <c r="B41" t="s">
-        <v>148</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -1907,10 +1949,10 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D42">
         <v>2</v>
@@ -1959,24 +2001,24 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -1990,10 +2032,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D3">
         <v>40</v>
@@ -2004,10 +2046,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D4">
         <v>30</v>
@@ -2018,10 +2060,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D5">
         <v>100</v>
@@ -2032,10 +2074,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D6">
         <v>30</v>
@@ -2046,13 +2088,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D7">
         <v>20</v>
@@ -2063,13 +2105,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -2080,10 +2122,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -2097,10 +2139,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -2111,10 +2153,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D11">
         <v>30</v>
@@ -2128,7 +2170,7 @@
         <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D12">
         <v>30</v>
@@ -2139,10 +2181,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D13">
         <v>5</v>
@@ -2185,13 +2227,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -2200,12 +2242,12 @@
         <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2214,7 +2256,7 @@
         <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -2228,7 +2270,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2237,7 +2279,7 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -2251,16 +2293,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>109</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>110</v>
-      </c>
       <c r="D4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -2274,7 +2316,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -2283,7 +2325,7 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -2320,21 +2362,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -2345,10 +2387,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3">
         <v>20</v>
@@ -2359,10 +2401,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -2373,10 +2415,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5">
         <v>40</v>
@@ -2387,10 +2429,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -2401,10 +2443,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C7">
         <v>20</v>
@@ -2415,10 +2457,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C8">
         <v>250</v>
@@ -2429,10 +2471,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C9">
         <v>20</v>
@@ -2443,10 +2485,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C10">
         <v>20</v>
@@ -2457,10 +2499,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C11">
         <v>20</v>
@@ -2474,7 +2516,7 @@
         <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C12">
         <v>20</v>
@@ -2510,21 +2552,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" t="s">
         <v>143</v>
-      </c>
-      <c r="B2" t="s">
-        <v>144</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -2540,7 +2582,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2CC720-2AFD-489A-814E-D75EB644CEB6}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2552,10 +2594,11 @@
     <col min="4" max="4" width="3.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -2563,12 +2606,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -2577,323 +2620,621 @@
       <c r="F1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="8" t="s">
         <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>169</v>
+        <v>72</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>72</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>183</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D2">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F2">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>170</v>
+      </c>
+      <c r="J2" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>184</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>178</v>
+      </c>
+      <c r="J3" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>185</v>
       </c>
       <c r="B4" s="5">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+      <c r="F4">
         <v>6</v>
       </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4">
-        <v>8</v>
+      <c r="G4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>175</v>
+      </c>
+      <c r="J4" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>186</v>
       </c>
       <c r="B5" s="5">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5" t="s">
+        <v>174</v>
+      </c>
+      <c r="J5" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B6" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>150</v>
+        <v>15</v>
       </c>
       <c r="D6">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E6">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F6">
-        <v>16</v>
-      </c>
-      <c r="G6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6">
-        <v>15</v>
+        <v>2</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B7" s="5">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
         <v>3</v>
       </c>
-      <c r="C7">
-        <v>200</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>16</v>
-      </c>
-      <c r="F7">
-        <v>20</v>
-      </c>
-      <c r="G7" t="s">
-        <v>75</v>
-      </c>
-      <c r="J7">
-        <v>40</v>
+      <c r="G7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B8" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>250</v>
+        <v>15</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E8">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F8">
-        <v>10</v>
-      </c>
-      <c r="G8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8">
-        <v>25</v>
+        <v>5</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B9" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>600</v>
+        <v>20</v>
       </c>
       <c r="D9">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E9">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>30</v>
-      </c>
-      <c r="G9" t="s">
-        <v>77</v>
-      </c>
-      <c r="H9" t="s">
-        <v>171</v>
-      </c>
-      <c r="I9" t="s">
-        <v>176</v>
-      </c>
-      <c r="J9">
-        <v>100</v>
+        <v>8</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B10" s="5">
         <v>2</v>
       </c>
       <c r="C10">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E10">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F10">
-        <v>16</v>
-      </c>
-      <c r="G10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" t="s">
-        <v>176</v>
+        <v>12</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10">
+        <v>25</v>
       </c>
       <c r="I10" t="s">
-        <v>171</v>
-      </c>
-      <c r="J10">
-        <v>30</v>
+        <v>178</v>
+      </c>
+      <c r="J10" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B11" s="5">
         <v>2</v>
       </c>
       <c r="C11">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F11">
-        <v>10</v>
-      </c>
-      <c r="G11" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" t="s">
-        <v>177</v>
-      </c>
-      <c r="J11">
-        <v>30</v>
+        <v>8</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11">
+        <v>25</v>
+      </c>
+      <c r="I11" t="s">
+        <v>175</v>
+      </c>
+      <c r="J11" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="B12" s="5">
         <v>2</v>
       </c>
       <c r="C12">
+        <v>25</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>11</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12">
+        <v>25</v>
+      </c>
+      <c r="I12" t="s">
+        <v>170</v>
+      </c>
+      <c r="J12" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B13" s="5">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>25</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <v>10</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13">
+        <v>25</v>
+      </c>
+      <c r="I13" t="s">
+        <v>174</v>
+      </c>
+      <c r="J13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="5">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>30</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>8</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="5">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>30</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>16</v>
+      </c>
+      <c r="F15">
+        <v>20</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>172</v>
+      </c>
+      <c r="B16" s="5">
+        <v>3</v>
+      </c>
+      <c r="C16">
         <v>35</v>
       </c>
-      <c r="D12">
+      <c r="D16">
         <v>2</v>
       </c>
-      <c r="E12">
+      <c r="E16">
         <v>4</v>
       </c>
-      <c r="F12">
+      <c r="F16">
+        <v>16</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16">
+        <v>50</v>
+      </c>
+      <c r="I16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>173</v>
+      </c>
+      <c r="B17" s="5">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>35</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>10</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17">
+        <v>50</v>
+      </c>
+      <c r="I17" t="s">
+        <v>175</v>
+      </c>
+      <c r="J17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B18" s="5">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>35</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18">
         <v>25</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G18" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J12">
-        <v>30</v>
+      <c r="H18">
+        <v>50</v>
+      </c>
+      <c r="I18" t="s">
+        <v>178</v>
+      </c>
+      <c r="J18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>176</v>
+      </c>
+      <c r="B19" s="5">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>35</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19">
+        <v>16</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19">
+        <v>50</v>
+      </c>
+      <c r="I19" t="s">
+        <v>174</v>
+      </c>
+      <c r="J19" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="5">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>25</v>
+      </c>
+      <c r="D20">
+        <v>10</v>
+      </c>
+      <c r="E20">
+        <v>15</v>
+      </c>
+      <c r="F20">
+        <v>16</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="5">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>150</v>
+      </c>
+      <c r="D21">
+        <v>15</v>
+      </c>
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="F21">
+        <v>35</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="H21">
+        <v>100</v>
+      </c>
+      <c r="I21" t="s">
+        <v>170</v>
+      </c>
+      <c r="J21" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J9">
-    <sortCondition ref="B2:B9"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N27">
+    <sortCondition ref="C2:C27"/>
+    <sortCondition ref="B2:B27"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2920,7 +3261,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2932,7 +3273,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2957,7 +3298,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -3037,7 +3378,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
@@ -3057,7 +3398,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B8" s="3">
         <v>2</v>
@@ -3077,7 +3418,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B9" s="3">
         <v>2</v>
@@ -3097,7 +3438,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
@@ -3117,7 +3458,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B11" s="3">
         <v>1</v>
@@ -3137,7 +3478,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B12" s="3">
         <v>1</v>
@@ -3157,7 +3498,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B13" s="3">
         <v>1</v>
@@ -3177,7 +3518,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
@@ -3197,7 +3538,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
@@ -3217,7 +3558,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
@@ -3237,7 +3578,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B17" s="3">
         <v>1</v>
@@ -3277,7 +3618,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -3286,15 +3627,15 @@
         <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3309,12 +3650,12 @@
         <v>80</v>
       </c>
       <c r="F2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -3329,12 +3670,12 @@
         <v>200</v>
       </c>
       <c r="F3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4">
         <v>6</v>
@@ -3349,12 +3690,12 @@
         <v>400</v>
       </c>
       <c r="F4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B5">
         <v>9</v>
@@ -3369,12 +3710,12 @@
         <v>850</v>
       </c>
       <c r="F5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6">
         <v>18</v>
@@ -3389,12 +3730,12 @@
         <v>3600</v>
       </c>
       <c r="F6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B7">
         <v>12</v>
@@ -3409,12 +3750,12 @@
         <v>1600</v>
       </c>
       <c r="F7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B8">
         <v>14</v>
@@ -3429,12 +3770,12 @@
         <v>7000</v>
       </c>
       <c r="F8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3449,12 +3790,12 @@
         <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3469,12 +3810,12 @@
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3489,12 +3830,12 @@
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3509,12 +3850,12 @@
         <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3529,7 +3870,7 @@
         <v>40</v>
       </c>
       <c r="F13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added spell cast duration.
</commit_message>
<xml_diff>
--- a/RougueQuest - Items and Enemies.xlsx
+++ b/RougueQuest - Items and Enemies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NTDLS\RougueQuest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2709436-E502-4B5F-984D-C088D7F66680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7426C6A5-2206-46B8-A6CE-1AE10BCAC9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="1128" windowWidth="17004" windowHeight="13356" xr2:uid="{C202AA48-B5B6-42E9-AECB-65F2B3A7610F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14160" activeTab="3" xr2:uid="{C202AA48-B5B6-42E9-AECB-65F2B3A7610F}"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="199">
   <si>
     <t>Name</t>
   </si>
@@ -340,21 +340,6 @@
     <t>Causes poisoning</t>
   </si>
   <si>
-    <t>Intelligence +5, 1 hour</t>
-  </si>
-  <si>
-    <t>Strength +15, 1 hour</t>
-  </si>
-  <si>
-    <t>Hitpoints +5, 1 hour</t>
-  </si>
-  <si>
-    <t>Dexterity +5, 1 hour</t>
-  </si>
-  <si>
-    <t>Strength +5, 1 hour</t>
-  </si>
-  <si>
     <t>Wooden Arrow</t>
   </si>
   <si>
@@ -517,9 +502,6 @@
     <t>Casts a fireball with splash damage withing 60 pixles</t>
   </si>
   <si>
-    <t>Armorclass +5, 1 hour</t>
-  </si>
-  <si>
     <t>Summons a hostile between level 1 and current level</t>
   </si>
   <si>
@@ -602,6 +584,60 @@
   </si>
   <si>
     <t>Metu Mortis</t>
+  </si>
+  <si>
+    <t>Cast Time</t>
+  </si>
+  <si>
+    <t>Ice Resistance</t>
+  </si>
+  <si>
+    <t>Fire Resistance</t>
+  </si>
+  <si>
+    <t>Electric Resistance</t>
+  </si>
+  <si>
+    <t>Earth Resistance</t>
+  </si>
+  <si>
+    <t>Reduces Ice damage by 1 half.</t>
+  </si>
+  <si>
+    <t>Reduces Fire damage by 1 half.</t>
+  </si>
+  <si>
+    <t>Reduces Electric damage by 1 half.</t>
+  </si>
+  <si>
+    <t>Reduces Earth damage by 1 half.</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>1 Hour</t>
+  </si>
+  <si>
+    <t>Armorclass +5</t>
+  </si>
+  <si>
+    <t>Intelligence +5</t>
+  </si>
+  <si>
+    <t>Hitpoints +5</t>
+  </si>
+  <si>
+    <t>Dexterity +5</t>
+  </si>
+  <si>
+    <t>Strength +5</t>
+  </si>
+  <si>
+    <t>1 hour</t>
+  </si>
+  <si>
+    <t>Strength +15</t>
   </si>
 </sst>
 </file>
@@ -645,7 +681,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -672,6 +708,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -988,7 +1025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAA9A541-9445-4B26-B43F-4615F42143DC}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
@@ -1008,10 +1045,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>83</v>
@@ -1034,7 +1071,7 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1057,7 +1094,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D3">
         <v>6</v>
@@ -1080,7 +1117,7 @@
         <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -1100,13 +1137,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B5" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D5">
         <v>10</v>
@@ -1129,7 +1166,7 @@
         <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1152,7 +1189,7 @@
         <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1175,7 +1212,7 @@
         <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1198,7 +1235,7 @@
         <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1221,7 +1258,7 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1244,7 +1281,7 @@
         <v>65</v>
       </c>
       <c r="B11" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1267,7 +1304,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1290,7 +1327,7 @@
         <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1313,7 +1350,7 @@
         <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1336,7 +1373,7 @@
         <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1359,7 +1396,7 @@
         <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1382,7 +1419,7 @@
         <v>88</v>
       </c>
       <c r="B17" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -1405,7 +1442,7 @@
         <v>89</v>
       </c>
       <c r="B18" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -1428,7 +1465,7 @@
         <v>47</v>
       </c>
       <c r="B19" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -1451,7 +1488,7 @@
         <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -1474,7 +1511,7 @@
         <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D21">
         <v>3</v>
@@ -1497,7 +1534,7 @@
         <v>90</v>
       </c>
       <c r="B22" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D22">
         <v>5</v>
@@ -1520,7 +1557,7 @@
         <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D23">
         <v>3</v>
@@ -1543,7 +1580,7 @@
         <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D24">
         <v>3</v>
@@ -1566,7 +1603,7 @@
         <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D25">
         <v>3</v>
@@ -1589,7 +1626,7 @@
         <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D26">
         <v>5</v>
@@ -1612,7 +1649,7 @@
         <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D27">
         <v>5</v>
@@ -1635,7 +1672,7 @@
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D28">
         <v>3</v>
@@ -1658,7 +1695,7 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D29">
         <v>3</v>
@@ -1681,7 +1718,7 @@
         <v>18</v>
       </c>
       <c r="B30" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D30">
         <v>3</v>
@@ -1704,7 +1741,7 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D31">
         <v>3</v>
@@ -1727,7 +1764,7 @@
         <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D32">
         <v>5</v>
@@ -1750,7 +1787,7 @@
         <v>84</v>
       </c>
       <c r="B33" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D33">
         <v>6</v>
@@ -1773,10 +1810,10 @@
         <v>62</v>
       </c>
       <c r="B34" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C34" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D34">
         <v>18</v>
@@ -1799,7 +1836,7 @@
         <v>28</v>
       </c>
       <c r="B35" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D35">
         <v>5</v>
@@ -1822,7 +1859,7 @@
         <v>12</v>
       </c>
       <c r="B36" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D36">
         <v>5</v>
@@ -1845,10 +1882,10 @@
         <v>54</v>
       </c>
       <c r="B37" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C37" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D37">
         <v>20</v>
@@ -1868,13 +1905,13 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B38" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C38" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D38">
         <v>28</v>
@@ -1897,10 +1934,10 @@
         <v>59</v>
       </c>
       <c r="B39" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C39" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D39">
         <v>25</v>
@@ -1923,10 +1960,10 @@
         <v>56</v>
       </c>
       <c r="B40" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C40" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D40">
         <v>30</v>
@@ -1946,10 +1983,10 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B41" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -1969,10 +2006,10 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B42" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D42">
         <v>2</v>
@@ -2001,22 +2038,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23A5046-8B05-44D0-A4EA-E6B6EFAC6BD3}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="E1" sqref="E1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2030,15 +2069,21 @@
         <v>93</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -2046,11 +2091,14 @@
       <c r="D2">
         <v>200</v>
       </c>
-      <c r="E2">
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -2060,27 +2108,36 @@
       <c r="D3">
         <v>40</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B4" t="s">
-        <v>158</v>
+        <v>192</v>
       </c>
       <c r="D4">
         <v>30</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B5" t="s">
         <v>92</v>
@@ -2088,27 +2145,36 @@
       <c r="D5">
         <v>100</v>
       </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>193</v>
       </c>
       <c r="D6">
         <v>30</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>191</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B7" t="s">
         <v>96</v>
@@ -2119,16 +2185,19 @@
       <c r="D7">
         <v>20</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>194</v>
       </c>
       <c r="C8" t="s">
         <v>95</v>
@@ -2136,16 +2205,22 @@
       <c r="D8">
         <v>10</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>191</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B9" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -2153,13 +2228,16 @@
       <c r="D9">
         <v>40</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B10" t="s">
         <v>98</v>
@@ -2167,59 +2245,158 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B11" t="s">
-        <v>102</v>
+        <v>195</v>
       </c>
       <c r="D11">
         <v>30</v>
       </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="E11" t="s">
+        <v>191</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B12" t="s">
-        <v>103</v>
-      </c>
-      <c r="D12">
+      <c r="B12" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="D12" s="10">
         <v>30</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>156</v>
-      </c>
-      <c r="B13" t="s">
-        <v>159</v>
-      </c>
-      <c r="D13">
-        <v>5</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
+      <c r="E12" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="F12" s="10">
+        <v>2</v>
+      </c>
+      <c r="G12" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="D13" s="10">
+        <v>5</v>
+      </c>
+      <c r="F13" s="10">
+        <v>3</v>
+      </c>
+      <c r="G13" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="D14" s="10">
+        <v>2</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="F14" s="10">
+        <v>2</v>
+      </c>
+      <c r="G14" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D15" s="10">
+        <v>2</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="F15" s="10">
+        <v>2</v>
+      </c>
+      <c r="G15" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="D16" s="10">
+        <v>2</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="F16" s="10">
+        <v>2</v>
+      </c>
+      <c r="G16" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D17" s="10">
+        <v>2</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="F17" s="10">
+        <v>2</v>
+      </c>
+      <c r="G17" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2253,7 +2430,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -2267,7 +2444,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2276,7 +2453,7 @@
         <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -2290,7 +2467,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2299,7 +2476,7 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -2313,16 +2490,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D4" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -2336,7 +2513,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -2345,7 +2522,7 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -2364,20 +2541,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61CAF6BD-7DF9-4703-AB96-7954B9A63A6D}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5546875" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2388,12 +2565,15 @@
         <v>93</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B2" t="s">
         <v>92</v>
@@ -2401,13 +2581,13 @@
       <c r="C2">
         <v>100</v>
       </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B3" t="s">
         <v>96</v>
@@ -2415,13 +2595,13 @@
       <c r="C3">
         <v>20</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B4" t="s">
         <v>95</v>
@@ -2429,13 +2609,13 @@
       <c r="C4">
         <v>10</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B5" t="s">
         <v>97</v>
@@ -2443,13 +2623,13 @@
       <c r="C5">
         <v>40</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B6" t="s">
         <v>98</v>
@@ -2457,91 +2637,109 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>193</v>
       </c>
       <c r="C7">
         <v>20</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
+        <v>198</v>
       </c>
       <c r="C8">
         <v>250</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="s">
+        <v>197</v>
+      </c>
+      <c r="E8">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>193</v>
       </c>
       <c r="C9">
         <v>20</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>197</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B10" t="s">
-        <v>101</v>
+        <v>194</v>
       </c>
       <c r="C10">
         <v>20</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>197</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B11" t="s">
-        <v>102</v>
+        <v>195</v>
       </c>
       <c r="C11">
         <v>20</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>197</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>103</v>
+        <v>196</v>
       </c>
       <c r="C12">
         <v>20</v>
       </c>
-      <c r="D12">
+      <c r="D12" t="s">
+        <v>197</v>
+      </c>
+      <c r="E12">
         <v>1</v>
       </c>
     </row>
@@ -2583,10 +2781,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -2605,7 +2803,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2649,15 +2847,15 @@
         <v>70</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
@@ -2681,15 +2879,15 @@
         <v>5</v>
       </c>
       <c r="I2" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="J2" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
@@ -2713,15 +2911,15 @@
         <v>5</v>
       </c>
       <c r="I3" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="J3" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B4" s="5">
         <v>1</v>
@@ -2745,15 +2943,15 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="J4" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B5" s="5">
         <v>1</v>
@@ -2777,10 +2975,10 @@
         <v>5</v>
       </c>
       <c r="I5" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="J5" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -2889,7 +3087,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B10" s="5">
         <v>2</v>
@@ -2913,15 +3111,15 @@
         <v>25</v>
       </c>
       <c r="I10" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="J10" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B11" s="5">
         <v>2</v>
@@ -2945,15 +3143,15 @@
         <v>25</v>
       </c>
       <c r="I11" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="J11" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B12" s="5">
         <v>2</v>
@@ -2977,15 +3175,15 @@
         <v>25</v>
       </c>
       <c r="I12" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="J12" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B13" s="5">
         <v>2</v>
@@ -3009,10 +3207,10 @@
         <v>25</v>
       </c>
       <c r="I13" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="J13" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -3069,7 +3267,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B16" s="5">
         <v>3</v>
@@ -3093,15 +3291,15 @@
         <v>50</v>
       </c>
       <c r="I16" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="J16" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B17" s="5">
         <v>3</v>
@@ -3125,15 +3323,15 @@
         <v>50</v>
       </c>
       <c r="I17" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="J17" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B18" s="5">
         <v>3</v>
@@ -3157,15 +3355,15 @@
         <v>50</v>
       </c>
       <c r="I18" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="J18" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B19" s="5">
         <v>3</v>
@@ -3189,10 +3387,10 @@
         <v>50</v>
       </c>
       <c r="I19" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="J19" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -3247,10 +3445,10 @@
         <v>100</v>
       </c>
       <c r="I21" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="J21" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -3320,7 +3518,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -3460,7 +3658,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
@@ -3480,7 +3678,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B11" s="3">
         <v>1</v>
@@ -3500,7 +3698,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B12" s="3">
         <v>1</v>
@@ -3520,7 +3718,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B13" s="3">
         <v>1</v>
@@ -3540,7 +3738,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
@@ -3560,7 +3758,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
@@ -3580,7 +3778,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
@@ -3600,7 +3798,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B17" s="3">
         <v>1</v>
@@ -3652,12 +3850,12 @@
         <v>91</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3672,12 +3870,12 @@
         <v>80</v>
       </c>
       <c r="F2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -3692,12 +3890,12 @@
         <v>200</v>
       </c>
       <c r="F3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B4">
         <v>6</v>
@@ -3712,12 +3910,12 @@
         <v>400</v>
       </c>
       <c r="F4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B5">
         <v>9</v>
@@ -3732,12 +3930,12 @@
         <v>850</v>
       </c>
       <c r="F5" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B6">
         <v>18</v>
@@ -3752,12 +3950,12 @@
         <v>3600</v>
       </c>
       <c r="F6" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B7">
         <v>12</v>
@@ -3772,12 +3970,12 @@
         <v>1600</v>
       </c>
       <c r="F7" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B8">
         <v>14</v>
@@ -3792,12 +3990,12 @@
         <v>7000</v>
       </c>
       <c r="F8" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3812,12 +4010,12 @@
         <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3832,12 +4030,12 @@
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3852,12 +4050,12 @@
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3872,12 +4070,12 @@
         <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3892,7 +4090,7 @@
         <v>40</v>
       </c>
       <c r="F13" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added store quantity and rarity populations.
</commit_message>
<xml_diff>
--- a/RougueQuest - Items and Enemies.xlsx
+++ b/RougueQuest - Items and Enemies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NTDLS\RougueQuest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7426C6A5-2206-46B8-A6CE-1AE10BCAC9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566416B1-7A3B-423F-8CC3-8B13A9FE9EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14160" activeTab="3" xr2:uid="{C202AA48-B5B6-42E9-AECB-65F2B3A7610F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14160" xr2:uid="{C202AA48-B5B6-42E9-AECB-65F2B3A7610F}"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="201">
   <si>
     <t>Name</t>
   </si>
@@ -496,15 +496,9 @@
     <t>Speed</t>
   </si>
   <si>
-    <t>Summon Monster</t>
-  </si>
-  <si>
     <t>Casts a fireball with splash damage withing 60 pixles</t>
   </si>
   <si>
-    <t>Summons a hostile between level 1 and current level</t>
-  </si>
-  <si>
     <t>Oil of Speed</t>
   </si>
   <si>
@@ -638,6 +632,18 @@
   </si>
   <si>
     <t>Strength +15</t>
+  </si>
+  <si>
+    <t>Summons a hostile between level 1 and level of wand</t>
+  </si>
+  <si>
+    <t>Summon Monster II</t>
+  </si>
+  <si>
+    <t>Summon Monster III</t>
+  </si>
+  <si>
+    <t>Summon Monster I</t>
   </si>
 </sst>
 </file>
@@ -1025,8 +1031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAA9A541-9445-4B26-B43F-4615F42143DC}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1048,7 +1054,7 @@
         <v>137</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>83</v>
@@ -1068,148 +1074,148 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>139</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>23</v>
+      <c r="E2" s="7">
+        <v>0</v>
       </c>
       <c r="F2">
         <v>10</v>
       </c>
       <c r="G2">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D3">
-        <v>6</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>37</v>
+        <v>2</v>
+      </c>
+      <c r="E3" s="7">
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="G3">
-        <v>115</v>
+        <v>10</v>
       </c>
       <c r="H3">
-        <v>80</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>138</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F4">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="G4">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="H4">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>180</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
         <v>138</v>
       </c>
-      <c r="C5" t="s">
-        <v>167</v>
-      </c>
       <c r="D5">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="F5">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="G5">
-        <v>160</v>
+        <v>115</v>
       </c>
       <c r="H5">
-        <v>750</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
         <v>138</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="G6">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="H6">
-        <v>5</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>178</v>
       </c>
       <c r="B7" t="s">
         <v>138</v>
       </c>
+      <c r="C7" t="s">
+        <v>165</v>
+      </c>
       <c r="D7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="F7">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="G7">
-        <v>35</v>
+        <v>160</v>
       </c>
       <c r="H7">
-        <v>5</v>
+        <v>750</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>138</v>
@@ -1221,10 +1227,10 @@
         <v>27</v>
       </c>
       <c r="F8">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="G8">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="H8">
         <v>5</v>
@@ -1232,7 +1238,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
         <v>138</v>
@@ -1244,10 +1250,10 @@
         <v>27</v>
       </c>
       <c r="F9">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G9">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="H9">
         <v>5</v>
@@ -1255,7 +1261,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
         <v>138</v>
@@ -1264,13 +1270,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10">
         <v>25</v>
       </c>
-      <c r="F10">
-        <v>15</v>
-      </c>
       <c r="G10">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="H10">
         <v>5</v>
@@ -1278,7 +1284,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
         <v>138</v>
@@ -1287,21 +1293,21 @@
         <v>1</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="F11">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="G11">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="H11">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
         <v>138</v>
@@ -1310,21 +1316,21 @@
         <v>1</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="F12">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G12">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="H12">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
         <v>138</v>
@@ -1336,7 +1342,7 @@
         <v>11</v>
       </c>
       <c r="F13">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="G13">
         <v>40</v>
@@ -1347,7 +1353,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
         <v>138</v>
@@ -1359,10 +1365,10 @@
         <v>11</v>
       </c>
       <c r="F14">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G14">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="H14">
         <v>10</v>
@@ -1370,7 +1376,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
         <v>138</v>
@@ -1382,10 +1388,10 @@
         <v>11</v>
       </c>
       <c r="F15">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="G15">
-        <v>115</v>
+        <v>40</v>
       </c>
       <c r="H15">
         <v>10</v>
@@ -1393,7 +1399,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
         <v>138</v>
@@ -1405,10 +1411,10 @@
         <v>11</v>
       </c>
       <c r="F16">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="G16">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="H16">
         <v>10</v>
@@ -1416,53 +1422,53 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>88</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
         <v>138</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>86</v>
+        <v>11</v>
       </c>
       <c r="F17">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="G17">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="H17">
-        <v>50</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
         <v>138</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>87</v>
+        <v>11</v>
       </c>
       <c r="F18">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G18">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="H18">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="B19" t="s">
         <v>138</v>
@@ -1471,53 +1477,53 @@
         <v>2</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="F19">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G19">
         <v>60</v>
       </c>
       <c r="H19">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="B20" t="s">
         <v>138</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="F20">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G20">
         <v>60</v>
       </c>
       <c r="H20">
-        <v>125</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s">
         <v>138</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F21">
         <v>15</v>
@@ -1526,21 +1532,21 @@
         <v>60</v>
       </c>
       <c r="H21">
-        <v>200</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
         <v>138</v>
       </c>
       <c r="D22">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F22">
         <v>15</v>
@@ -1549,12 +1555,12 @@
         <v>60</v>
       </c>
       <c r="H22">
-        <v>400</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
         <v>138</v>
@@ -1563,44 +1569,44 @@
         <v>3</v>
       </c>
       <c r="E23" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23">
         <v>15</v>
       </c>
-      <c r="F23">
-        <v>30</v>
-      </c>
       <c r="G23">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="H23">
-        <v>40</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="B24" t="s">
         <v>138</v>
       </c>
       <c r="D24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E24" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24">
         <v>15</v>
       </c>
-      <c r="F24">
-        <v>20</v>
-      </c>
       <c r="G24">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="H24">
-        <v>40</v>
+        <v>400</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
         <v>138</v>
@@ -1612,10 +1618,10 @@
         <v>15</v>
       </c>
       <c r="F25">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="G25">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="H25">
         <v>40</v>
@@ -1623,16 +1629,16 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
         <v>138</v>
       </c>
       <c r="D26">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="F26">
         <v>20</v>
@@ -1641,81 +1647,81 @@
         <v>80</v>
       </c>
       <c r="H26">
-        <v>200</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B27" t="s">
         <v>138</v>
       </c>
       <c r="D27">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="F27">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="G27">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="H27">
-        <v>325</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
         <v>138</v>
       </c>
       <c r="D28">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="F28">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="G28">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="H28">
-        <v>60</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B29" t="s">
         <v>138</v>
       </c>
       <c r="D29">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="F29">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="G29">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="H29">
-        <v>60</v>
+        <v>325</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B30" t="s">
         <v>138</v>
@@ -1724,21 +1730,21 @@
         <v>3</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F30">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G30">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="H30">
-        <v>100</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
         <v>138</v>
@@ -1747,30 +1753,30 @@
         <v>3</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F31">
+        <v>50</v>
+      </c>
+      <c r="G31">
+        <v>115</v>
+      </c>
+      <c r="H31">
         <v>60</v>
-      </c>
-      <c r="G31">
-        <v>120</v>
-      </c>
-      <c r="H31">
-        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B32" t="s">
         <v>138</v>
       </c>
       <c r="D32">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F32">
         <v>50</v>
@@ -1779,257 +1785,257 @@
         <v>95</v>
       </c>
       <c r="H32">
-        <v>250</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>84</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>138</v>
       </c>
       <c r="D33">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>85</v>
+        <v>19</v>
       </c>
       <c r="F33">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G33">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="H33">
-        <v>450</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="B34" t="s">
         <v>138</v>
       </c>
-      <c r="C34" t="s">
-        <v>166</v>
-      </c>
       <c r="D34">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="F34">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="G34">
-        <v>200</v>
+        <v>95</v>
       </c>
       <c r="H34">
-        <v>4000</v>
+        <v>250</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="B35" t="s">
         <v>138</v>
       </c>
       <c r="D35">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="F35">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="G35">
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="H35">
-        <v>40</v>
+        <v>450</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="B36" t="s">
         <v>138</v>
       </c>
+      <c r="C36" t="s">
+        <v>164</v>
+      </c>
       <c r="D36">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="F36">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="G36">
-        <v>95</v>
+        <v>200</v>
       </c>
       <c r="H36">
-        <v>60</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="B37" t="s">
         <v>138</v>
       </c>
-      <c r="C37" t="s">
-        <v>162</v>
-      </c>
       <c r="D37">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="F37">
-        <v>105</v>
+        <v>25</v>
       </c>
       <c r="G37">
-        <v>155</v>
+        <v>45</v>
       </c>
       <c r="H37">
-        <v>4500</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>179</v>
+        <v>12</v>
       </c>
       <c r="B38" t="s">
         <v>138</v>
       </c>
-      <c r="C38" t="s">
-        <v>166</v>
-      </c>
       <c r="D38">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="F38">
-        <v>120</v>
+        <v>20</v>
       </c>
       <c r="G38">
-        <v>180</v>
+        <v>95</v>
       </c>
       <c r="H38">
-        <v>3600</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B39" t="s">
         <v>138</v>
       </c>
       <c r="C39" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="D39">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F39">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="G39">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="H39">
-        <v>3000</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>177</v>
       </c>
       <c r="B40" t="s">
         <v>138</v>
       </c>
       <c r="C40" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D40">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F40">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="G40">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="H40">
-        <v>3200</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>139</v>
+        <v>59</v>
       </c>
       <c r="B41" t="s">
-        <v>140</v>
+        <v>138</v>
+      </c>
+      <c r="C41" t="s">
+        <v>149</v>
       </c>
       <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41" s="7">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="F41">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="G41">
-        <v>9</v>
+        <v>145</v>
       </c>
       <c r="H41">
-        <v>40</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>141</v>
+        <v>56</v>
       </c>
       <c r="B42" t="s">
-        <v>140</v>
+        <v>138</v>
+      </c>
+      <c r="C42" t="s">
+        <v>160</v>
       </c>
       <c r="D42">
-        <v>2</v>
-      </c>
-      <c r="E42" s="7">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="F42">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="G42">
-        <v>10</v>
+        <v>150</v>
       </c>
       <c r="H42">
-        <v>200</v>
+        <v>3200</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H40">
-    <sortCondition ref="E2:E40"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H42">
+    <sortCondition ref="E2:E42"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2041,7 +2047,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F1"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2069,10 +2075,10 @@
         <v>93</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>83</v>
@@ -2083,7 +2089,7 @@
         <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -2120,13 +2126,13 @@
         <v>143</v>
       </c>
       <c r="B4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D4">
         <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -2157,13 +2163,13 @@
         <v>145</v>
       </c>
       <c r="B6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D6">
         <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -2197,7 +2203,7 @@
         <v>148</v>
       </c>
       <c r="B8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C8" t="s">
         <v>95</v>
@@ -2206,7 +2212,7 @@
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F8">
         <v>2</v>
@@ -2257,13 +2263,13 @@
         <v>150</v>
       </c>
       <c r="B11" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D11">
         <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F11">
         <v>2</v>
@@ -2277,13 +2283,13 @@
         <v>69</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D12" s="10">
         <v>30</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F12" s="10">
         <v>2</v>
@@ -2294,10 +2300,10 @@
     </row>
     <row r="13" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>151</v>
+        <v>200</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>153</v>
+        <v>197</v>
       </c>
       <c r="D13" s="10">
         <v>5</v>
@@ -2311,16 +2317,16 @@
     </row>
     <row r="14" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D14" s="10">
         <v>2</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F14" s="10">
         <v>2</v>
@@ -2331,16 +2337,16 @@
     </row>
     <row r="15" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D15" s="10">
         <v>2</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F15" s="10">
         <v>2</v>
@@ -2351,16 +2357,16 @@
     </row>
     <row r="16" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D16" s="10">
         <v>2</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F16" s="10">
         <v>2</v>
@@ -2371,17 +2377,17 @@
     </row>
     <row r="17" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B17" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D17" s="10">
+        <v>2</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="D17" s="10">
-        <v>2</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>191</v>
-      </c>
       <c r="F17" s="10">
         <v>2</v>
       </c>
@@ -2389,8 +2395,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D18" s="10">
+        <v>10</v>
+      </c>
+      <c r="F18" s="10">
+        <v>3</v>
+      </c>
+      <c r="G18" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D19" s="10">
+        <v>20</v>
+      </c>
+      <c r="F19" s="10">
+        <v>3</v>
+      </c>
+      <c r="G19" s="10">
+        <v>3</v>
+      </c>
+    </row>
     <row r="20" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -2430,7 +2468,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -2453,7 +2491,7 @@
         <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -2476,7 +2514,7 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -2499,7 +2537,7 @@
         <v>102</v>
       </c>
       <c r="D4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -2522,7 +2560,7 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -2543,7 +2581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61CAF6BD-7DF9-4703-AB96-7954B9A63A6D}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2565,7 +2603,7 @@
         <v>93</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>83</v>
@@ -2573,7 +2611,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B2" t="s">
         <v>92</v>
@@ -2587,7 +2625,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B3" t="s">
         <v>96</v>
@@ -2601,7 +2639,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B4" t="s">
         <v>95</v>
@@ -2615,7 +2653,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B5" t="s">
         <v>97</v>
@@ -2646,13 +2684,13 @@
         <v>143</v>
       </c>
       <c r="B7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C7">
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -2660,16 +2698,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C8">
         <v>250</v>
       </c>
       <c r="D8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E8">
         <v>3</v>
@@ -2680,13 +2718,13 @@
         <v>145</v>
       </c>
       <c r="B9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C9">
         <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -2697,13 +2735,13 @@
         <v>148</v>
       </c>
       <c r="B10" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C10">
         <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -2711,16 +2749,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B11" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C11">
         <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -2731,13 +2769,13 @@
         <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C12">
         <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -2847,15 +2885,15 @@
         <v>70</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
@@ -2879,15 +2917,15 @@
         <v>5</v>
       </c>
       <c r="I2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
@@ -2911,15 +2949,15 @@
         <v>5</v>
       </c>
       <c r="I3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B4" s="5">
         <v>1</v>
@@ -2943,15 +2981,15 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B5" s="5">
         <v>1</v>
@@ -2975,10 +3013,10 @@
         <v>5</v>
       </c>
       <c r="I5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -3087,7 +3125,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B10" s="5">
         <v>2</v>
@@ -3111,15 +3149,15 @@
         <v>25</v>
       </c>
       <c r="I10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B11" s="5">
         <v>2</v>
@@ -3143,15 +3181,15 @@
         <v>25</v>
       </c>
       <c r="I11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J11" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B12" s="5">
         <v>2</v>
@@ -3175,15 +3213,15 @@
         <v>25</v>
       </c>
       <c r="I12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B13" s="5">
         <v>2</v>
@@ -3207,10 +3245,10 @@
         <v>25</v>
       </c>
       <c r="I13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -3267,7 +3305,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B16" s="5">
         <v>3</v>
@@ -3291,15 +3329,15 @@
         <v>50</v>
       </c>
       <c r="I16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B17" s="5">
         <v>3</v>
@@ -3323,15 +3361,15 @@
         <v>50</v>
       </c>
       <c r="I17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J17" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B18" s="5">
         <v>3</v>
@@ -3355,15 +3393,15 @@
         <v>50</v>
       </c>
       <c r="I18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J18" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B19" s="5">
         <v>3</v>
@@ -3387,10 +3425,10 @@
         <v>50</v>
       </c>
       <c r="I19" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J19" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -3445,10 +3483,10 @@
         <v>100</v>
       </c>
       <c r="I21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J21" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>